<commit_message>
tidy up energy and radar
</commit_message>
<xml_diff>
--- a/05-Energy/Energy Data.xlsx
+++ b/05-Energy/Energy Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fion\Desktop\ICL\Y2\EOY Project\EOY-Project\05-Energy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F210CB5-F584-4621-AEA5-1D98E4CB179E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BAF6CCE-7DA2-4AE0-B827-2D65179A034E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{FCB29C0A-5EFC-414A-AA0D-4A7847955301}"/>
+    <workbookView xWindow="4845" yWindow="1680" windowWidth="21600" windowHeight="11505" activeTab="2" xr2:uid="{FCB29C0A-5EFC-414A-AA0D-4A7847955301}"/>
   </bookViews>
   <sheets>
     <sheet name="Battery characteristics" sheetId="1" r:id="rId1"/>
@@ -9913,7 +9913,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="1" refreshError="1"/>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -10510,7 +10510,7 @@
   <dimension ref="A1:S21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:S21"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11486,7 +11486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1A2B781-BE6C-4575-9B93-F35E4AFFDE84}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
       <selection activeCell="U25" sqref="U25"/>
     </sheetView>
   </sheetViews>
@@ -11736,7 +11736,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B87ED69-90AC-4EEA-A63B-BBA63DEFDF6F}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>

</xml_diff>